<commit_message>
chore(quotation): update quotation template layout
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模报价单.xlsx
+++ b/backend/templates/quotation/美菱改模报价单.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/work/jiuhuan/backend/templates/quotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\changdq\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D124C101-7CC0-EE4D-844E-94DE53A6307C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B8ACE9-12FE-4619-8D1B-FEE276B68A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="40960" windowHeight="22420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="改模报价" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +565,78 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -575,85 +647,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,25 +674,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="absolute">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>117476</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>403926</xdr:colOff>
+      <xdr:colOff>488625</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>230325</xdr:rowOff>
+      <xdr:rowOff>220800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2">
+        <xdr:cNvPr id="4" name="图片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FED8B75C-F18B-4355-BBD8-1961335302BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5928EED-AF4F-4358-BB09-5F49E3E926BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -702,7 +702,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:alphaModFix amt="50000"/>
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -715,23 +714,23 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4210051" y="247650"/>
-          <a:ext cx="1512000" cy="1440000"/>
+          <a:off x="4210050" y="238125"/>
+          <a:ext cx="1584000" cy="1440000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
+    <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -769,9 +768,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -804,9 +803,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,9 +855,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1019,398 +1052,398 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:I23"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:9" ht="25" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="26"/>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="34"/>
-    </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="34"/>
-    </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="1:9" ht="20" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="34"/>
-    </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="34"/>
-    </row>
-    <row r="20" spans="1:9" ht="20" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="34"/>
-    </row>
-    <row r="21" spans="1:9" ht="20" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="34"/>
-    </row>
-    <row r="22" spans="1:9" ht="20" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="34"/>
-    </row>
-    <row r="23" spans="1:9" ht="20" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10" t="s">
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="34"/>
-    </row>
-    <row r="24" spans="1:9" ht="20" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" ht="20" customHeight="1">
-      <c r="A25" s="9" t="s">
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" ht="27" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
@@ -1418,198 +1451,136 @@
       <c r="G26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="8"/>
-    </row>
-    <row r="27" spans="1:9" ht="24.5" customHeight="1">
-      <c r="A27" s="14" t="s">
+      <c r="H26" s="24"/>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="1:9" ht="20" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="28"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" ht="20" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="16"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="9" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" ht="18" customHeight="1">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="11"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="12" t="s">
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" ht="20" customHeight="1">
-      <c r="A34" s="9" t="s">
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="34"/>
+    </row>
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
@@ -1626,6 +1597,68 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore(quotation): tweak quotation template
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模报价单.xlsx
+++ b/backend/templates/quotation/美菱改模报价单.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\changdq\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B8ACE9-12FE-4619-8D1B-FEE276B68A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07429D28-9B09-4328-85E3-1B29470F0396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,14 +565,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,16 +586,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -616,44 +634,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,9 +683,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>488625</xdr:colOff>
+      <xdr:colOff>477811</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>220800</xdr:rowOff>
+      <xdr:rowOff>213600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -697,7 +697,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -715,7 +715,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4210050" y="238125"/>
-          <a:ext cx="1584000" cy="1440000"/>
+          <a:ext cx="1573186" cy="1432800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1069,381 +1069,381 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="32"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="32"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="32"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="32"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="32"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="32"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="32"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="9"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="32"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="9"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="32"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="32"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="32"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="9"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="32"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="32"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="32"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="32"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="25"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="25"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
@@ -1451,136 +1451,198 @@
       <c r="G26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="28"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="10"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="11"/>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="11"/>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="8"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="33" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="34"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9" t="s">
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="9"/>
-      <c r="I34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="31"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="78">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
@@ -1597,71 +1659,10 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(quotation): update quotation template
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模报价单.xlsx
+++ b/backend/templates/quotation/美菱改模报价单.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\changdq\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/work/jiuhuan/backend/templates/quotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07429D28-9B09-4328-85E3-1B29470F0396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4096C7-F3B5-AA4E-BE45-F4080687A191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="改模报价" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,7 +549,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -565,6 +565,72 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,83 +643,20 @@
     <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,7 +686,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>477811</xdr:colOff>
+      <xdr:colOff>579411</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>213600</xdr:rowOff>
     </xdr:to>
@@ -728,9 +731,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -768,9 +771,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -803,26 +806,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -855,26 +841,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1052,398 +1021,398 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="7.375" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:9" ht="30" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="25" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="20" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="9" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="20" customHeight="1">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="20" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
+    <row r="8" spans="1:9" ht="20" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="20" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" ht="20" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="30"/>
+    </row>
+    <row r="11" spans="1:9" ht="20" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" ht="20" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" ht="20" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
+    <row r="14" spans="1:9" ht="20" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="33" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10" t="s">
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" ht="20" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="33" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" ht="20" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="4" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="20" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="33" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" ht="20" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="33" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" ht="20" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="4" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="33" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10" t="s">
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" ht="20" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="4" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10" t="s">
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" spans="1:9" ht="20" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="4" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="33" t="s">
         <v>34</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10" t="s">
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="30"/>
+    </row>
+    <row r="22" spans="1:9" ht="20" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="33" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10" t="s">
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23" spans="1:9" ht="20" customHeight="1">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="33" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="1:9" ht="20" customHeight="1">
+      <c r="A24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="1:9" ht="20" customHeight="1">
+      <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="9" t="s">
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="1:9" ht="27" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
@@ -1451,198 +1420,136 @@
       <c r="G26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="14" t="s">
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="24.5" customHeight="1">
+      <c r="A27" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="9" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" ht="20" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="14" t="s">
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" ht="20" customHeight="1">
+      <c r="A29" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="16"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9" t="s">
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="11"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="12" t="s">
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="9" t="s">
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" ht="20" customHeight="1">
+      <c r="A34" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1">
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
@@ -1659,6 +1566,68 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
chore(quotation): update completion template file
</commit_message>
<xml_diff>
--- a/backend/templates/quotation/美菱改模报价单.xlsx
+++ b/backend/templates/quotation/美菱改模报价单.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changun/work/jiuhuan/backend/templates/quotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\changdq\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415E82C5-8239-4842-8067-F74029818D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E3FDD2-AFA2-4554-99D1-F62BFAB28109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="40960" windowHeight="22420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="改模报价" sheetId="1" r:id="rId1"/>
@@ -213,10 +213,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="177" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,7 +565,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -574,40 +575,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="31" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,53 +614,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -674,6 +627,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,6 +643,57 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,16 +716,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>135255</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>831215</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>67310</xdr:rowOff>
+      <xdr:colOff>1075055</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -739,8 +752,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4060190" y="390525"/>
-          <a:ext cx="1369695" cy="1403985"/>
+          <a:off x="4257675" y="17145"/>
+          <a:ext cx="1351280" cy="1391285"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -753,9 +766,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -793,9 +806,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -828,9 +841,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -863,9 +893,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1043,37 +1090,37 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
-    </row>
-    <row r="2" spans="1:9" ht="25" customHeight="1">
-      <c r="A2" s="29" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
@@ -1085,40 +1132,40 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" ht="20" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="30" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" ht="20" customHeight="1">
-      <c r="A5" s="29" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="10"/>
@@ -1128,12 +1175,12 @@
       <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" ht="20" customHeight="1">
-      <c r="A6" s="29" t="s">
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
@@ -1143,10 +1190,10 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="31"/>
-    </row>
-    <row r="7" spans="1:9" ht="20" customHeight="1">
-      <c r="A7" s="29" t="s">
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="10"/>
@@ -1164,67 +1211,67 @@
         <v>14</v>
       </c>
       <c r="H7" s="10"/>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20" customHeight="1">
-      <c r="A8" s="29"/>
+    <row r="8" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="20" customHeight="1">
-      <c r="A9" s="29"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="20" customHeight="1">
-      <c r="A10" s="29"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="20" customHeight="1">
-      <c r="A11" s="29"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="20" customHeight="1">
-      <c r="A12" s="29"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="38"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" ht="20" customHeight="1">
-      <c r="A13" s="29" t="s">
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="38"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="10"/>
@@ -1242,12 +1289,12 @@
         <v>20</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20" customHeight="1">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
         <v>21</v>
@@ -1257,12 +1304,12 @@
         <v>22</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" ht="20" customHeight="1">
-      <c r="A15" s="29"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
         <v>23</v>
@@ -1272,12 +1319,12 @@
         <v>24</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="20" customHeight="1">
-      <c r="A16" s="29"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="38"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
         <v>25</v>
@@ -1287,12 +1334,12 @@
         <v>26</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" ht="20" customHeight="1">
-      <c r="A17" s="29"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
         <v>27</v>
@@ -1302,12 +1349,12 @@
         <v>28</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="20" customHeight="1">
-      <c r="A18" s="29"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
         <v>29</v>
@@ -1317,12 +1364,12 @@
         <v>28</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1">
-      <c r="A19" s="29"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="38"/>
+    </row>
+    <row r="19" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10" t="s">
         <v>30</v>
@@ -1332,12 +1379,12 @@
         <v>31</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="20" customHeight="1">
-      <c r="A20" s="29"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
         <v>32</v>
@@ -1347,12 +1394,12 @@
         <v>33</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="20" customHeight="1">
-      <c r="A21" s="29"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="38"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
         <v>34</v>
@@ -1362,12 +1409,12 @@
         <v>35</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" ht="20" customHeight="1">
-      <c r="A22" s="29"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
         <v>36</v>
@@ -1377,12 +1424,12 @@
         <v>22</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" ht="20" customHeight="1">
-      <c r="A23" s="29"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10" t="s">
         <v>37</v>
@@ -1392,12 +1439,12 @@
         <v>38</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" ht="20" customHeight="1">
-      <c r="A24" s="29" t="s">
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="38"/>
+    </row>
+    <row r="24" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="10"/>
@@ -1407,12 +1454,12 @@
       <c r="F24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" ht="20" customHeight="1">
-      <c r="A25" s="29" t="s">
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="10"/>
@@ -1424,12 +1471,12 @@
       <c r="F25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" ht="27" customHeight="1">
-      <c r="A26" s="29" t="s">
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="10"/>
@@ -1438,28 +1485,28 @@
       <c r="E26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="33" t="s">
+      <c r="F26" s="41"/>
+      <c r="G26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" ht="24.5" customHeight="1">
-      <c r="A27" s="34" t="s">
+      <c r="H26" s="39"/>
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" ht="24.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="36"/>
-    </row>
-    <row r="28" spans="1:9" ht="20" customHeight="1">
-      <c r="A28" s="29" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="10"/>
@@ -1471,23 +1518,23 @@
       <c r="H28" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" ht="20" customHeight="1">
-      <c r="A29" s="34" t="s">
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="36"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" customHeight="1">
-      <c r="A30" s="29" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="10"/>
@@ -1499,10 +1546,10 @@
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="31"/>
-    </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1">
-      <c r="A31" s="29" t="s">
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B31" s="10"/>
@@ -1514,10 +1561,10 @@
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="31"/>
-    </row>
-    <row r="32" spans="1:9" ht="18" customHeight="1">
-      <c r="A32" s="29"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1527,113 +1574,51 @@
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="31"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" customHeight="1">
-      <c r="A33" s="29"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
-    </row>
-    <row r="34" spans="1:9" ht="20" customHeight="1">
-      <c r="A34" s="7" t="s">
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8" t="s">
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" ht="30" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="5"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="G35:I35"/>
@@ -1650,11 +1635,73 @@
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="A29:I29"/>
     <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>